<commit_message>
started added hero instances
</commit_message>
<xml_diff>
--- a/hero_bullets.xlsx
+++ b/hero_bullets.xlsx
@@ -29637,7 +29637,7 @@
         <v>0.0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
@@ -29676,7 +29676,7 @@
       </c>
       <c r="N2" s="12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O2" s="12">
         <f t="shared" ref="O2:O21" si="6">MIN(INT(E2*16),255)</f>
@@ -29706,7 +29706,7 @@
         <v>0.0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="1">
         <v>1.0</v>
@@ -29745,7 +29745,7 @@
       </c>
       <c r="N3" s="12">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O3" s="12">
         <f t="shared" si="6"/>
@@ -29775,7 +29775,7 @@
         <v>5.0</v>
       </c>
       <c r="C4" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D4" s="1">
         <v>1.0</v>
@@ -29814,7 +29814,7 @@
       </c>
       <c r="N4" s="12">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4" s="12">
         <f t="shared" si="6"/>
@@ -29844,7 +29844,7 @@
         <v>5.0</v>
       </c>
       <c r="C5" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D5" s="1">
         <v>1.0</v>
@@ -29883,7 +29883,7 @@
       </c>
       <c r="N5" s="12">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="6"/>
@@ -29913,7 +29913,7 @@
         <v>5.0</v>
       </c>
       <c r="C6" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D6" s="1">
         <v>1.0</v>
@@ -29952,7 +29952,7 @@
       </c>
       <c r="N6" s="12">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="12">
         <f t="shared" si="6"/>
@@ -29982,7 +29982,7 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D7" s="1">
         <v>1.0</v>
@@ -30021,7 +30021,7 @@
       </c>
       <c r="N7" s="12">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="12">
         <f t="shared" si="6"/>
@@ -30051,7 +30051,7 @@
         <v>5.0</v>
       </c>
       <c r="C8" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D8" s="1">
         <v>1.0</v>
@@ -30090,7 +30090,7 @@
       </c>
       <c r="N8" s="12">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="12">
         <f t="shared" si="6"/>
@@ -30120,7 +30120,7 @@
         <v>5.0</v>
       </c>
       <c r="C9" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D9" s="1">
         <v>1.0</v>
@@ -30159,7 +30159,7 @@
       </c>
       <c r="N9" s="12">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9" s="12">
         <f t="shared" si="6"/>
@@ -30183,7 +30183,7 @@
         <v>5.0</v>
       </c>
       <c r="C10" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D10" s="1">
         <v>1.0</v>
@@ -30222,7 +30222,7 @@
       </c>
       <c r="N10" s="12">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="12">
         <f t="shared" si="6"/>
@@ -30246,7 +30246,7 @@
         <v>0.0</v>
       </c>
       <c r="C11" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D11" s="1">
         <v>1.0</v>
@@ -30285,7 +30285,7 @@
       </c>
       <c r="N11" s="12">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O11" s="12">
         <f t="shared" si="6"/>
@@ -30305,7 +30305,7 @@
         <v>0.0</v>
       </c>
       <c r="C12" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="1">
         <v>1.0</v>
@@ -30344,7 +30344,7 @@
       </c>
       <c r="N12" s="12">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" s="12">
         <f t="shared" si="6"/>
@@ -30364,7 +30364,7 @@
         <v>5.0</v>
       </c>
       <c r="C13" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D13" s="1">
         <v>1.0</v>
@@ -30403,7 +30403,7 @@
       </c>
       <c r="N13" s="12">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" s="12">
         <f t="shared" si="6"/>
@@ -30423,7 +30423,7 @@
         <v>5.0</v>
       </c>
       <c r="C14" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D14" s="1">
         <v>1.0</v>
@@ -30462,7 +30462,7 @@
       </c>
       <c r="N14" s="12">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="12">
         <f t="shared" si="6"/>
@@ -30482,7 +30482,7 @@
         <v>5.0</v>
       </c>
       <c r="C15" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D15" s="1">
         <v>1.0</v>
@@ -30521,7 +30521,7 @@
       </c>
       <c r="N15" s="12">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" s="12">
         <f t="shared" si="6"/>
@@ -30541,7 +30541,7 @@
         <v>5.0</v>
       </c>
       <c r="C16" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D16" s="1">
         <v>1.0</v>
@@ -30580,7 +30580,7 @@
       </c>
       <c r="N16" s="12">
         <f t="shared" si="33"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" s="12">
         <f t="shared" si="6"/>
@@ -30600,7 +30600,7 @@
         <v>5.0</v>
       </c>
       <c r="C17" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D17" s="1">
         <v>1.0</v>
@@ -30639,7 +30639,7 @@
       </c>
       <c r="N17" s="12">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O17" s="12">
         <f t="shared" si="6"/>
@@ -30659,7 +30659,7 @@
         <v>5.0</v>
       </c>
       <c r="C18" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D18" s="1">
         <v>1.0</v>
@@ -30698,7 +30698,7 @@
       </c>
       <c r="N18" s="12">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" s="12">
         <f t="shared" si="6"/>
@@ -30718,7 +30718,7 @@
         <v>5.0</v>
       </c>
       <c r="C19" s="1">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D19" s="1">
         <v>1.0</v>
@@ -30757,7 +30757,7 @@
       </c>
       <c r="N19" s="12">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O19" s="12">
         <f t="shared" si="6"/>
@@ -30777,7 +30777,7 @@
         <v>0.0</v>
       </c>
       <c r="C20" s="1">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="D20" s="1">
         <v>2.0</v>
@@ -30816,7 +30816,7 @@
       </c>
       <c r="N20" s="12">
         <f t="shared" si="41"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O20" s="12">
         <f t="shared" si="6"/>
@@ -30836,7 +30836,7 @@
         <v>0.0</v>
       </c>
       <c r="C21" s="1">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="D21" s="1">
         <v>2.0</v>
@@ -30875,7 +30875,7 @@
       </c>
       <c r="N21" s="12">
         <f t="shared" si="43"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O21" s="12">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
destroy enemy and hero simple game loop
</commit_message>
<xml_diff>
--- a/hero_bullets.xlsx
+++ b/hero_bullets.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
   <si>
     <t>BulletTypes</t>
   </si>
@@ -123,7 +123,13 @@
     <t>int8_t</t>
   </si>
   <si>
+    <t>Wings_Blade_Special</t>
+  </si>
+  <si>
     <t>Alient_Buster</t>
+  </si>
+  <si>
+    <t>Alient_Buster_Special</t>
   </si>
   <si>
     <t>Musketeer</t>
@@ -710,7 +716,7 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="1">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
@@ -724,7 +730,7 @@
       </c>
       <c r="G2" s="2">
         <f t="shared" ref="G2:G4" si="2">INT(C2*16)</f>
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="8" t="b">
@@ -764,7 +770,7 @@
         <v>0.05</v>
       </c>
       <c r="C3" s="1">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" s="1">
         <v>1.0</v>
@@ -778,7 +784,7 @@
       </c>
       <c r="G3" s="2">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="8" t="b">
@@ -818,7 +824,7 @@
         <v>0.05</v>
       </c>
       <c r="C4" s="1">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="D4" s="1">
         <v>1.0</v>
@@ -832,7 +838,7 @@
       </c>
       <c r="G4" s="2">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="8" t="b">
@@ -31860,7 +31866,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1">
         <v>5.0</v>
@@ -31911,7 +31917,7 @@
       </c>
       <c r="P4" s="13">
         <f t="array" ref="P4">INDEX(SourceTypes!$B$2:$B999,MATCH(A4,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q4" s="13">
         <f t="shared" ref="Q4:R4" si="9">MIN(INT(B4*16),255)</f>
@@ -31943,7 +31949,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1">
         <v>5.0</v>
@@ -31994,7 +32000,7 @@
       </c>
       <c r="P5" s="13">
         <f t="array" ref="P5">INDEX(SourceTypes!$B$2:$B999,MATCH(A5,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="13">
         <f t="shared" ref="Q5:R5" si="11">MIN(INT(B5*16),255)</f>
@@ -32026,7 +32032,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1">
         <v>5.0</v>
@@ -32077,7 +32083,7 @@
       </c>
       <c r="P6" s="13">
         <f t="array" ref="P6">INDEX(SourceTypes!$B$2:$B999,MATCH(A6,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q6" s="13">
         <f t="shared" ref="Q6:R6" si="13">MIN(INT(B6*16),255)</f>
@@ -32109,7 +32115,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1">
         <v>5.0</v>
@@ -32160,7 +32166,7 @@
       </c>
       <c r="P7" s="13">
         <f t="array" ref="P7">INDEX(SourceTypes!$B$2:$B999,MATCH(A7,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q7" s="13">
         <f t="shared" ref="Q7:R7" si="15">MIN(INT(B7*16),255)</f>
@@ -32192,7 +32198,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1">
         <v>5.0</v>
@@ -32243,7 +32249,7 @@
       </c>
       <c r="P8" s="13">
         <f t="array" ref="P8">INDEX(SourceTypes!$B$2:$B999,MATCH(A8,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q8" s="13">
         <f t="shared" ref="Q8:R8" si="17">MIN(INT(B8*16),255)</f>
@@ -32275,7 +32281,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1">
         <v>5.0</v>
@@ -32326,7 +32332,7 @@
       </c>
       <c r="P9" s="13">
         <f t="array" ref="P9">INDEX(SourceTypes!$B$2:$B999,MATCH(A9,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q9" s="13">
         <f t="shared" ref="Q9:R9" si="19">MIN(INT(B9*16),255)</f>
@@ -32358,7 +32364,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1">
         <v>5.0</v>
@@ -32409,7 +32415,7 @@
       </c>
       <c r="P10" s="13">
         <f t="array" ref="P10">INDEX(SourceTypes!$B$2:$B999,MATCH(A10,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="13">
         <f t="shared" ref="Q10:R10" si="21">MIN(INT(B10*16),255)</f>
@@ -32441,7 +32447,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1">
         <v>0.0</v>
@@ -32518,7 +32524,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1">
         <v>0.0</v>
@@ -32595,7 +32601,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1">
         <v>5.0</v>
@@ -32646,7 +32652,7 @@
       </c>
       <c r="P13" s="13">
         <f t="array" ref="P13">INDEX(SourceTypes!$B$2:$B999,MATCH(A13,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" ref="Q13:R13" si="27">MIN(INT(B13*16),255)</f>
@@ -32672,7 +32678,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1">
         <v>5.0</v>
@@ -32723,7 +32729,7 @@
       </c>
       <c r="P14" s="13">
         <f t="array" ref="P14">INDEX(SourceTypes!$B$2:$B999,MATCH(A14,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" ref="Q14:R14" si="29">MIN(INT(B14*16),255)</f>
@@ -32749,7 +32755,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>5.0</v>
@@ -32800,7 +32806,7 @@
       </c>
       <c r="P15" s="13">
         <f t="array" ref="P15">INDEX(SourceTypes!$B$2:$B999,MATCH(A15,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="13">
         <f t="shared" ref="Q15:R15" si="31">MIN(INT(B15*16),255)</f>
@@ -32826,7 +32832,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1">
         <v>5.0</v>
@@ -32877,7 +32883,7 @@
       </c>
       <c r="P16" s="13">
         <f t="array" ref="P16">INDEX(SourceTypes!$B$2:$B999,MATCH(A16,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="13">
         <f t="shared" ref="Q16:R16" si="33">MIN(INT(B16*16),255)</f>
@@ -32903,7 +32909,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>5.0</v>
@@ -32954,7 +32960,7 @@
       </c>
       <c r="P17" s="13">
         <f t="array" ref="P17">INDEX(SourceTypes!$B$2:$B999,MATCH(A17,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" ref="Q17:R17" si="35">MIN(INT(B17*16),255)</f>
@@ -32980,7 +32986,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1">
         <v>5.0</v>
@@ -33031,7 +33037,7 @@
       </c>
       <c r="P18" s="13">
         <f t="array" ref="P18">INDEX(SourceTypes!$B$2:$B999,MATCH(A18,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="13">
         <f t="shared" ref="Q18:R18" si="37">MIN(INT(B18*16),255)</f>
@@ -33057,7 +33063,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1">
         <v>5.0</v>
@@ -33108,7 +33114,7 @@
       </c>
       <c r="P19" s="13">
         <f t="array" ref="P19">INDEX(SourceTypes!$B$2:$B999,MATCH(A19,SourceTypes!$A$2:$A999,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="13">
         <f t="shared" ref="Q19:R19" si="39">MIN(INT(B19*16),255)</f>
@@ -33134,7 +33140,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1">
         <v>0.0</v>
@@ -33211,7 +33217,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1">
         <v>0.0</v>
@@ -55808,7 +55814,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.75"/>
+    <col customWidth="1" min="1" max="1" width="17.63"/>
     <col customWidth="1" min="2" max="2" width="11.0"/>
     <col customWidth="1" min="3" max="3" width="22.38"/>
     <col customWidth="1" min="4" max="4" width="19.13"/>
@@ -55825,10 +55831,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="12"/>
       <c r="F1" s="4" t="s">
@@ -55854,7 +55860,7 @@
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(SourceBulletTypes!$A$2:$A964,A2)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="9" t="b">
@@ -55862,7 +55868,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>11</v>
@@ -55870,7 +55876,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="9">
         <v>1.0</v>
@@ -55881,7 +55887,7 @@
       </c>
       <c r="D3" s="2">
         <f>COUNTIF(SourceBulletTypes!$A$2:$A964,A3)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="9" t="b">
@@ -55889,7 +55895,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>11</v>
@@ -55897,7 +55903,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9">
         <v>2.0</v>
@@ -55918,7 +55924,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9">
         <v>3.0</v>
@@ -55938,15 +55944,37 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4.0</v>
+      </c>
+      <c r="C6" s="2">
+        <f>IFNA(MATCH(A6,SourceBulletTypes!$A$2:$A964,0)-1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <f>COUNTIF(SourceBulletTypes!$A$2:$A964,A6)</f>
+        <v>7</v>
+      </c>
       <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5.0</v>
+      </c>
+      <c r="C7" s="2">
+        <f>IFNA(MATCH(A7,SourceBulletTypes!$A$2:$A964,0)-1,0)</f>
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <f>COUNTIF(SourceBulletTypes!$A$2:$A964,A7)</f>
+        <v>7</v>
+      </c>
       <c r="E7" s="12"/>
     </row>
     <row r="8">

</xml_diff>